<commit_message>
Check list de calidad de enero
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/Checklist_Calidad_160128.xlsx
+++ b/Proyectos/2016/Calidad/Checklist_Calidad_160128.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" state="visible" r:id="rId2"/>
@@ -255,10 +255,10 @@
     <t>¿Tiene definido el nombre del cliente atendido?</t>
   </si>
   <si>
-    <t>¿Se tiene especificada la necesidad del cliente?</t>
+    <t>¿Se tiene especificada el personal que atendió la solicitud?</t>
   </si>
   <si>
-    <t>¿La carta de aceptación tiene las respuestas de servicio por parte del cliente, es decir el cliente definió el tipo de servicio y trato recibido?</t>
+    <t>¿Se tiene la fecha de realización?</t>
   </si>
   <si>
     <t>¿Se tiene especificado el software/hardware entregado?</t>
@@ -734,7 +734,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="5" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1056,8 +1056,8 @@
   </sheetPr>
   <dimension ref="1:36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -19697,7 +19697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="26" t="str">
         <f aca="false">Física!A3</f>
         <v>Elementos de Configuración</v>
@@ -19744,7 +19744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="26" t="str">
         <f aca="false">Funcional!A3</f>
         <v>Entregables</v>
@@ -19789,7 +19789,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="B26:B29 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -19888,7 +19888,7 @@
     </row>
     <row r="7" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
         <v>13</v>
       </c>
@@ -19902,7 +19902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39"/>
       <c r="B10" s="39"/>
       <c r="C10" s="42" t="s">
@@ -19916,7 +19916,7 @@
       </c>
       <c r="F10" s="41"/>
     </row>
-    <row r="11" s="38" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="44" t="n">
         <v>1</v>
       </c>
@@ -19930,7 +19930,7 @@
       <c r="E11" s="44"/>
       <c r="F11" s="45"/>
     </row>
-    <row r="12" s="38" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="44" t="n">
         <v>2</v>
       </c>
@@ -19944,7 +19944,7 @@
       <c r="E12" s="44"/>
       <c r="F12" s="45"/>
     </row>
-    <row r="13" s="38" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="44" t="n">
         <v>3</v>
       </c>
@@ -19958,7 +19958,7 @@
       <c r="E13" s="44"/>
       <c r="F13" s="45"/>
     </row>
-    <row r="14" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="44" t="n">
         <v>4</v>
       </c>
@@ -19972,7 +19972,7 @@
       <c r="E14" s="44"/>
       <c r="F14" s="45"/>
     </row>
-    <row r="15" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="44" t="n">
         <v>5</v>
       </c>
@@ -19986,7 +19986,7 @@
       <c r="E15" s="44"/>
       <c r="F15" s="45"/>
     </row>
-    <row r="16" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44" t="n">
         <v>6</v>
       </c>
@@ -20000,7 +20000,7 @@
       <c r="E16" s="44"/>
       <c r="F16" s="45"/>
     </row>
-    <row r="17" s="38" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="47" t="n">
         <v>1</v>
       </c>
@@ -20014,7 +20014,7 @@
       <c r="E17" s="49"/>
       <c r="F17" s="50"/>
     </row>
-    <row r="18" s="38" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="47" t="n">
         <v>2</v>
       </c>
@@ -20028,7 +20028,7 @@
       <c r="E18" s="49"/>
       <c r="F18" s="50"/>
     </row>
-    <row r="19" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="49" t="n">
         <v>3</v>
       </c>
@@ -20042,7 +20042,7 @@
       <c r="E19" s="49"/>
       <c r="F19" s="50"/>
     </row>
-    <row r="20" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="n">
         <v>4</v>
       </c>
@@ -20056,7 +20056,7 @@
       <c r="E20" s="49"/>
       <c r="F20" s="50"/>
     </row>
-    <row r="21" s="38" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="44" t="n">
         <v>7</v>
       </c>
@@ -20070,38 +20070,10 @@
       </c>
       <c r="F21" s="53"/>
     </row>
-    <row r="22" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0"/>
-    </row>
-    <row r="23" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="0"/>
-      <c r="F23" s="0"/>
-    </row>
-    <row r="24" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-    </row>
-    <row r="25" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-      <c r="E25" s="0"/>
-      <c r="F25" s="0"/>
-    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39" t="s">
         <v>44</v>
@@ -20564,8 +20536,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20929,7 +20901,7 @@
       <c r="E27" s="64"/>
       <c r="F27" s="65"/>
     </row>
-    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="64" t="n">
         <v>3</v>
       </c>
@@ -21089,7 +21061,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="B26:B29 C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21191,8 +21163,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="B26:B29 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>